<commit_message>
minor change in brands, Razer to Medion
</commit_message>
<xml_diff>
--- a/master_data/brands.xlsx
+++ b/master_data/brands.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72f513831c36f08e/Trabajos/PCComponentes/master_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72f513831c36f08e/Trabajos/laptops-data-cleaning/master_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{F03DF94E-D359-48CD-87F9-48A9FAC68495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4106E28D-D634-4863-BC52-D7A31E9C2EC6}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{F03DF94E-D359-48CD-87F9-48A9FAC68495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13FD92FB-2B37-4923-B105-068EBC0AA576}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E71BC730-6E9A-46F5-94B7-90A8F9A5F8C2}"/>
   </bookViews>
@@ -184,10 +184,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -562,50 +558,50 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
minor changes, HP brand fixed
</commit_message>
<xml_diff>
--- a/master_data/brands.xlsx
+++ b/master_data/brands.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72f513831c36f08e/Trabajos/laptops-data-cleaning/master_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{F03DF94E-D359-48CD-87F9-48A9FAC68495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13FD92FB-2B37-4923-B105-068EBC0AA576}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{F03DF94E-D359-48CD-87F9-48A9FAC68495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82CE8A6B-6491-469C-A430-A45355D3AB8B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E71BC730-6E9A-46F5-94B7-90A8F9A5F8C2}"/>
   </bookViews>
@@ -184,6 +184,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -526,199 +530,199 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>28</v>
@@ -726,18 +730,18 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes in models
</commit_message>
<xml_diff>
--- a/master_data/brands.xlsx
+++ b/master_data/brands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/72f513831c36f08e/Trabajos/laptops-data-cleaning/master_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="8_{F03DF94E-D359-48CD-87F9-48A9FAC68495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82CE8A6B-6491-469C-A430-A45355D3AB8B}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="8_{F03DF94E-D359-48CD-87F9-48A9FAC68495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{05BA34C1-3E90-40E3-BA15-D5202E765059}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E71BC730-6E9A-46F5-94B7-90A8F9A5F8C2}"/>
   </bookViews>
@@ -706,15 +706,15 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>28</v>
@@ -722,26 +722,26 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B31" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>